<commit_message>
EPBDS-7689 remove System.out.println from tests and replace it with counter
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ExternalConditions_AdditionalCases.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ExternalConditions_AdditionalCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\conditionReferencess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2DA67F-526F-48C2-B02D-0F306B879796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B020EE79-2B5A-4A2F-8FFD-1889F3934CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="195" windowWidth="27360" windowHeight="15090" xr2:uid="{87148A64-2808-4D00-A1E5-2239350ABB0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87148A64-2808-4D00-A1E5-2239350ABB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="171">
   <si>
     <t>String</t>
   </si>
@@ -228,9 +228,6 @@
     <t>(param2&lt;&gt;c2param)&amp;&amp;param2&lt;min</t>
   </si>
   <si>
-    <t>Rules  Double[] mytest(Integer param1, String param2)</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>contains(lengthArr, calcLegth(strParam))</t>
   </si>
   <si>
-    <t>=System.out.println(intArr[0])</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>Void aParam</t>
   </si>
   <si>
-    <t>Test mytest</t>
-  </si>
-  <si>
     <t>=aParam; lengthArr</t>
   </si>
   <si>
@@ -487,6 +478,72 @@
   </si>
   <si>
     <t>//**Long field + arr in condition</t>
+  </si>
+  <si>
+    <t>Datatype Counter</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>times1</t>
+  </si>
+  <si>
+    <t>Rules  Double[] mytest(Integer param1, String param2, Counter count)</t>
+  </si>
+  <si>
+    <t>=times += 1</t>
+  </si>
+  <si>
+    <t>=times1 += 1</t>
+  </si>
+  <si>
+    <t>= aParam;  aParam; lengthArr</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult mytestWrapper(Integer param1, String param2)</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>= new Counter()</t>
+  </si>
+  <si>
+    <t>= $Counter.times</t>
+  </si>
+  <si>
+    <t>= mytest(param1, param2, $Counter)</t>
+  </si>
+  <si>
+    <t>Row1Times</t>
+  </si>
+  <si>
+    <t>Row2Times</t>
+  </si>
+  <si>
+    <t>= $Counter.times1</t>
+  </si>
+  <si>
+    <t>Test mytestWrapper</t>
+  </si>
+  <si>
+    <t>_res_.$Result</t>
+  </si>
+  <si>
+    <t>_res_.$Row2Times</t>
+  </si>
+  <si>
+    <t>_res_.$Row1Times</t>
   </si>
 </sst>
 </file>
@@ -629,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -659,6 +716,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -675,12 +734,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -692,6 +745,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB961AA-EEF0-4203-A4D7-1E7675658564}">
-  <dimension ref="C2:P139"/>
+  <dimension ref="C2:P147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,8 +1077,8 @@
     <col min="3" max="3" width="67.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="26.42578125" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="21.85546875" customWidth="1" collapsed="1"/>
@@ -1030,17 +1089,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="26"/>
       <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="24"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -1102,17 +1161,17 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -1206,14 +1265,14 @@
     </row>
     <row r="18" spans="3:9" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
@@ -1305,29 +1364,29 @@
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>19</v>
@@ -1337,15 +1396,15 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" s="26"/>
+      <c r="C32" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="28"/>
       <c r="E32" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>52</v>
@@ -1365,7 +1424,7 @@
         <v>48</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>51</v>
@@ -1385,7 +1444,7 @@
         <v>49</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>50</v>
@@ -1425,7 +1484,7 @@
         <v>250</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2">
@@ -1434,23 +1493,23 @@
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="C40" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="27"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="6" t="s">
         <v>16</v>
       </c>
@@ -1460,25 +1519,25 @@
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="27"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G42" s="6"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="27"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>51</v>
@@ -1510,13 +1569,13 @@
         <v>200</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
@@ -1527,13 +1586,13 @@
         <v>500</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
@@ -1549,10 +1608,10 @@
       <c r="F48" s="10"/>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="24"/>
+      <c r="C49" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="26"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
     </row>
@@ -1581,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -1591,7 +1650,7 @@
         <v>201</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -1654,7 +1713,7 @@
         <v>217</v>
       </c>
       <c r="G61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
@@ -1668,772 +1727,859 @@
         <v>1000</v>
       </c>
       <c r="G62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C65" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C66" s="16"/>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" t="s">
+        <v>159</v>
+      </c>
+      <c r="G68" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="G69" t="s">
+        <v>150</v>
+      </c>
+      <c r="H69" t="s">
+        <v>151</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="G70" t="s">
+        <v>150</v>
+      </c>
+      <c r="H70" t="s">
+        <v>152</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C76" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="29"/>
+      <c r="E76" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" s="34"/>
+      <c r="G76" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C65" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C67" s="27" t="s">
+      <c r="F77" s="29"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C78" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78" s="29"/>
+      <c r="G78" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-    </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C68" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="27"/>
-      <c r="E68" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="F68" s="34"/>
-      <c r="G68" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C69" s="27" t="s">
+      <c r="H79" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C80" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F69" s="27"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-    </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C70" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E70" s="27" t="s">
+      <c r="D80" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E80" s="6">
+        <v>1</v>
+      </c>
+      <c r="F80" s="6">
+        <v>2</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H80" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="F70" s="27"/>
-      <c r="G70" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H70" s="6"/>
-    </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C71" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E72" s="6">
-        <v>1</v>
-      </c>
-      <c r="F72" s="6">
-        <v>2</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C73" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E73" s="6">
-        <v>3</v>
-      </c>
-      <c r="F73" s="6">
-        <v>4</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C76" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-    </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C77" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C78" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C79" s="6">
-        <v>100</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C81" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="12"/>
-    </row>
-    <row r="82" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D82" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E82" s="27"/>
-      <c r="F82" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G82" s="13"/>
-    </row>
-    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D83" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E83" s="27"/>
-      <c r="F83" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G83" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E81" s="6">
+        <v>3</v>
+      </c>
+      <c r="F81" s="6">
+        <v>4</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G84" s="12"/>
+      <c r="C84" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C85" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D85" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="E85" s="27"/>
-      <c r="F85" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G85" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F85" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="G85" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E87" s="10"/>
-    </row>
-    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D88" s="11"/>
-      <c r="E88" s="12"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
+      <c r="C87" s="6">
+        <v>100</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
     </row>
     <row r="89" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C89" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E89" s="12"/>
-    </row>
-    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E90" s="12"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G90" s="13"/>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C91" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E91" s="10"/>
+        <v>89</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="29"/>
+      <c r="F91" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" s="12"/>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C92" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G92" s="12"/>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D93" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E93" s="29"/>
+      <c r="F93" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D92" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E92" s="12"/>
-    </row>
-    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C93" s="10"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-    </row>
-    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D94" s="23"/>
-      <c r="E94" s="12"/>
+      <c r="G93" s="12"/>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C95" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E95" s="12"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C96" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>126</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D96" s="11"/>
       <c r="E96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
     </row>
     <row r="97" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C97" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>125</v>
+        <v>88</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="E97" s="12"/>
     </row>
     <row r="98" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C98" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D98" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E98" s="10"/>
+      <c r="E98" s="12"/>
+    </row>
+    <row r="99" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C99" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C100" s="16" t="s">
-        <v>133</v>
-      </c>
+      <c r="C100" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E100" s="12"/>
+    </row>
+    <row r="101" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C101" s="10"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
     </row>
     <row r="102" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C102" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="23"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="23"/>
-      <c r="K102" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="L102" s="32"/>
-      <c r="M102" s="33"/>
+      <c r="C102" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102" s="25"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C103" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D103" s="27"/>
-      <c r="E103" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G103" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K103" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L103" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M103" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="C103" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C104" s="6" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E104" s="6">
-        <v>3</v>
-      </c>
-      <c r="F104" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K104" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L104" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M104" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C105" s="6" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E105" s="6">
-        <v>4</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="K105" s="6">
-        <v>20</v>
-      </c>
-      <c r="L105" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M105" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
+      <c r="C106" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="E106" s="10"/>
-      <c r="F106" s="10"/>
-    </row>
-    <row r="107" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="10"/>
     </row>
     <row r="108" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C108" s="16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C110" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
+      <c r="C110" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D110" s="25"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="25"/>
+      <c r="G110" s="25"/>
+      <c r="K110" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="L110" s="32"/>
+      <c r="M110" s="33"/>
     </row>
     <row r="111" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C111" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D111" s="27"/>
+      <c r="C111" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D111" s="29"/>
       <c r="E111" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F111" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="I111" s="27"/>
+        <v>94</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K111" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L111" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M111" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="112" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C112" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E112" s="6">
         <v>3</v>
       </c>
-      <c r="F112" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G112" s="30"/>
-      <c r="H112" s="6">
-        <v>556</v>
-      </c>
-      <c r="I112" s="6">
-        <v>3885</v>
-      </c>
-    </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F112" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K112" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L112" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M112" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="113" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C113" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E113" s="6">
         <v>4</v>
       </c>
-      <c r="F113" s="29" t="s">
+      <c r="F113" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K113" s="6">
+        <v>20</v>
+      </c>
+      <c r="L113" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M113" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C114" s="10"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="10"/>
+    </row>
+    <row r="115" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+    </row>
+    <row r="116" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C116" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C118" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+      <c r="G118" s="29"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+    </row>
+    <row r="119" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C119" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D119" s="29"/>
+      <c r="E119" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F119" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G119" s="29"/>
+      <c r="H119" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I119" s="29"/>
+    </row>
+    <row r="120" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C120" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E120" s="6">
+        <v>3</v>
+      </c>
+      <c r="F120" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G120" s="36"/>
+      <c r="H120" s="6">
+        <v>556</v>
+      </c>
+      <c r="I120" s="6">
+        <v>3885</v>
+      </c>
+    </row>
+    <row r="121" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C121" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E121" s="6">
+        <v>4</v>
+      </c>
+      <c r="F121" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G121" s="36"/>
+      <c r="H121" s="6">
+        <v>853</v>
+      </c>
+      <c r="I121" s="6">
+        <v>6556</v>
+      </c>
+    </row>
+    <row r="124" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C124" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="G113" s="30"/>
-      <c r="H113" s="6">
+      <c r="D124" s="26"/>
+      <c r="E124" s="26"/>
+      <c r="F124" s="6"/>
+    </row>
+    <row r="125" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C125" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C126" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C127" s="6">
+        <v>20</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="128" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C128" s="6">
+        <v>200</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F128" s="6">
         <v>853</v>
       </c>
-      <c r="I113" s="6">
-        <v>6556</v>
-      </c>
-    </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C116" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="6"/>
-    </row>
-    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C117" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117" s="6" t="s">
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C129" s="6">
+        <v>200</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C136" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="D136" s="27"/>
+      <c r="E136" s="27"/>
+      <c r="F136" s="27"/>
+      <c r="G136" s="27"/>
+    </row>
+    <row r="137" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C137" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G137" s="2"/>
+    </row>
+    <row r="138" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C138" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G138" s="2"/>
+    </row>
+    <row r="139" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C139" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G139" s="2"/>
+    </row>
+    <row r="140" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C140" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C141" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D141" s="20">
+        <v>73051</v>
+      </c>
+      <c r="E141" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F141" t="s">
+        <v>138</v>
+      </c>
+      <c r="G141" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D144" s="25"/>
+      <c r="E144" s="25"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="25"/>
+      <c r="H144" s="25"/>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C145" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D145" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="118" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C118" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D118" s="6" t="s">
+      <c r="E145" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F145" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G145" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H145" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="146" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C146" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D146" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E118" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="119" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C119" s="6">
-        <v>20</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E119" s="6" t="s">
+      <c r="E146" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F146" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G146" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H146" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C147" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F119" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="120" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C120" s="6">
-        <v>200</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F120" s="6">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="121" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C121" s="6">
-        <v>200</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="125" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C125" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="128" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C128" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
-      <c r="G128" s="25"/>
-    </row>
-    <row r="129" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C129" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G129" s="2"/>
-    </row>
-    <row r="130" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C130" s="2" t="s">
+      <c r="D147" s="22">
+        <v>43831</v>
+      </c>
+      <c r="E147" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F147" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G147" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F130" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G130" s="2"/>
-    </row>
-    <row r="131" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C131" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G131" s="2"/>
-    </row>
-    <row r="132" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C132" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="133" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C133" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D133" s="20">
-        <v>73051</v>
-      </c>
-      <c r="E133" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="F133" t="s">
-        <v>141</v>
-      </c>
-      <c r="G133" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="136" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C136" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D136" s="23"/>
-      <c r="E136" s="23"/>
-      <c r="F136" s="23"/>
-      <c r="G136" s="23"/>
-      <c r="H136" s="23"/>
-    </row>
-    <row r="137" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C137" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D137" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E137" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F137" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G137" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H137" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="138" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C138" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D138" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E138" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F138" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G138" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H138" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="139" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C139" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D139" s="22">
-        <v>43831</v>
-      </c>
-      <c r="E139" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F139" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G139" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H139" s="22">
+      <c r="H147" s="22">
         <v>73051</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="F112:G112"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C128:G128"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="K102:M102"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="C110:I110"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C136:H136"/>
+    <mergeCell ref="F120:G120"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="K110:M110"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="C118:I118"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="F119:G119"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C144:H144"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="H2:I2"/>
@@ -2446,9 +2592,9 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="E78:F78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2460,7 +2606,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>